<commit_message>
Rename/update/add notebook "Estimate intensity ratio — its dependency of beta parameters, *.ipynb"
</commit_message>
<xml_diff>
--- a/Data/Simulated He beta parameters, TDSE.xlsx
+++ b/Data/Simulated He beta parameters, TDSE.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daehyun/Documents/FERMI 20144077 Ueda/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daehyun/Google Drive (daehyun.you.tohoku@gmail.com)/FERMI 20144077 Ueda/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57208731-227A-1048-B216-06F4FB020CFA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFA8CE5-5607-7048-BEF8-6BEF1060B4FE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="500" windowWidth="33600" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39120" yWindow="7960" windowWidth="33600" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>coeff_s</t>
   </si>
@@ -51,6 +51,9 @@
   <si>
     <t>Int ratio</t>
   </si>
+  <si>
+    <t>Ref int ratio</t>
+  </si>
 </sst>
 </file>
 
@@ -60,7 +63,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
-    <numFmt numFmtId="169" formatCode="0E+00"/>
+    <numFmt numFmtId="167" formatCode="0E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -130,16 +133,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
     <dxf>
       <font>
         <b val="0"/>
@@ -158,46 +161,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="166" formatCode="0.000E+00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -317,7 +280,67 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="169" formatCode="0E+00"/>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000E+00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0E+00"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -394,21 +417,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B47044FF-AC89-0543-AD60-B1147F8E9F3A}" name="Table1" displayName="Table1" ref="A1:J11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J11" xr:uid="{0EC1BCB9-238E-CA48-ACD3-0EA01E4EA545}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{7101E157-D5E7-8A4B-946A-B6E74DCEAF70}" name="Photon (eV)" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{2C495F66-30F6-9E4E-967C-79653BE3E862}" name="Int_w (W/cm2)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{4A7E127C-EFDF-BA42-91B6-BF2941CAA564}" name="Int_2w (W/cm2)" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{A9B82F4B-28EE-1A4C-8401-0C70DF7BE54A}" name="Int ratio" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B47044FF-AC89-0543-AD60-B1147F8E9F3A}" name="Table1" displayName="Table1" ref="A1:K11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K11" xr:uid="{0EC1BCB9-238E-CA48-ACD3-0EA01E4EA545}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{7101E157-D5E7-8A4B-946A-B6E74DCEAF70}" name="Photon (eV)" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{2C495F66-30F6-9E4E-967C-79653BE3E862}" name="Int_w (W/cm2)" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{4A7E127C-EFDF-BA42-91B6-BF2941CAA564}" name="Int_2w (W/cm2)" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{A9B82F4B-28EE-1A4C-8401-0C70DF7BE54A}" name="Int ratio" dataDxfId="7">
       <calculatedColumnFormula>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E147D237-6FD7-BC49-ADAC-9C5266B4F422}" name="coeff_s" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{7E13E67C-A2E5-2D47-B80D-F11EA6BC5C66}" name="coeff_p" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{6B4B88FE-6405-544F-9CFC-AA06E63FA7F5}" name="coeff_d" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{230DDAD2-C284-B846-A4D5-C2493A94250E}" name="eta_s" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{56A46975-3382-8843-A4F4-D16289575AA4}" name="eta_p" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{38EE8EFC-DB03-764C-BC34-018626DCDA09}" name="eta_d" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{2F256323-95A5-1B46-9EB0-05620C78964E}" name="Ref int ratio" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Int ratio]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{E147D237-6FD7-BC49-ADAC-9C5266B4F422}" name="coeff_s" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{7E13E67C-A2E5-2D47-B80D-F11EA6BC5C66}" name="coeff_p" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{6B4B88FE-6405-544F-9CFC-AA06E63FA7F5}" name="coeff_d" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{230DDAD2-C284-B846-A4D5-C2493A94250E}" name="eta_s" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{56A46975-3382-8843-A4F4-D16289575AA4}" name="eta_p" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{38EE8EFC-DB03-764C-BC34-018626DCDA09}" name="eta_d" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -714,11 +740,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -727,11 +753,12 @@
     <col min="2" max="2" width="15" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="8.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="15" customWidth="1"/>
+    <col min="6" max="8" width="9.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.1640625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -744,32 +771,35 @@
       <c r="D1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>14.3</v>
       </c>
@@ -783,32 +813,36 @@
         <f>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</f>
         <v>1.1661903789690601E-8</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="14">
+        <f>Table1[[#This Row],[Int ratio]]</f>
+        <v>1.1661903789690601E-8</v>
+      </c>
+      <c r="F2" s="9">
         <v>3.2200000000000002E-3</v>
       </c>
-      <c r="F2" s="9">
+      <c r="G2" s="9">
         <v>1.14E-2</v>
       </c>
-      <c r="G2" s="9">
+      <c r="H2" s="9">
         <v>-1.09E-2</v>
       </c>
-      <c r="H2" s="8">
+      <c r="I2" s="8">
         <v>5.36</v>
       </c>
-      <c r="I2" s="8">
+      <c r="J2" s="8">
         <v>2.2599999999999998</v>
       </c>
-      <c r="J2" s="8">
+      <c r="K2" s="8">
         <v>0</v>
       </c>
-      <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>15</v>
       </c>
@@ -822,32 +856,36 @@
         <f>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</f>
         <v>1.1575836902790226E-8</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="14">
+        <f>Table1[[#This Row],[Int ratio]]</f>
+        <v>1.1575836902790226E-8</v>
+      </c>
+      <c r="F3" s="9">
         <v>2.5300000000000001E-3</v>
       </c>
-      <c r="F3" s="9">
+      <c r="G3" s="9">
         <v>1.0500000000000001E-2</v>
       </c>
-      <c r="G3" s="9">
+      <c r="H3" s="9">
         <v>-1.0200000000000001E-2</v>
       </c>
-      <c r="H3" s="8">
+      <c r="I3" s="8">
         <v>5.22</v>
       </c>
-      <c r="I3" s="8">
+      <c r="J3" s="8">
         <v>2.19</v>
       </c>
-      <c r="J3" s="8">
+      <c r="K3" s="8">
         <v>0</v>
       </c>
-      <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>15.9</v>
       </c>
@@ -861,32 +899,36 @@
         <f>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</f>
         <v>1.1180339887498947E-8</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="14">
+        <f>Table1[[#This Row],[Int ratio]]</f>
+        <v>1.1180339887498947E-8</v>
+      </c>
+      <c r="F4" s="9">
         <v>1.7700000000000001E-3</v>
       </c>
-      <c r="F4" s="9">
+      <c r="G4" s="9">
         <v>9.4400000000000005E-3</v>
       </c>
-      <c r="G4" s="9">
+      <c r="H4" s="9">
         <v>-9.2800000000000001E-3</v>
       </c>
-      <c r="H4" s="8">
+      <c r="I4" s="8">
         <v>5.07</v>
       </c>
-      <c r="I4" s="8">
+      <c r="J4" s="8">
         <v>2.12</v>
       </c>
-      <c r="J4" s="8">
+      <c r="K4" s="8">
         <v>0</v>
       </c>
-      <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>16</v>
       </c>
@@ -900,32 +942,36 @@
         <f>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</f>
         <v>1.1224972160321824E-8</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="14">
+        <f>Table1[[#This Row],[Int ratio]]</f>
+        <v>1.1224972160321824E-8</v>
+      </c>
+      <c r="F5" s="9">
         <v>1.6900000000000001E-3</v>
       </c>
-      <c r="F5" s="9">
+      <c r="G5" s="9">
         <v>9.3299999999999998E-3</v>
       </c>
-      <c r="G5" s="9">
+      <c r="H5" s="9">
         <v>-9.1699999999999993E-3</v>
       </c>
-      <c r="H5" s="8">
+      <c r="I5" s="8">
         <v>5.0599999999999996</v>
       </c>
-      <c r="I5" s="8">
+      <c r="J5" s="8">
         <v>2.11</v>
       </c>
-      <c r="J5" s="8">
+      <c r="K5" s="8">
         <v>0</v>
       </c>
-      <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>17</v>
       </c>
@@ -939,32 +985,36 @@
         <f>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</f>
         <v>1.0862780491200217E-8</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="14">
+        <f>Table1[[#This Row],[Int ratio]]</f>
+        <v>1.0862780491200217E-8</v>
+      </c>
+      <c r="F6" s="9">
         <v>9.859999999999999E-4</v>
       </c>
-      <c r="F6" s="9">
+      <c r="G6" s="9">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="G6" s="9">
+      <c r="H6" s="9">
         <v>-8.2400000000000008E-3</v>
       </c>
-      <c r="H6" s="8">
+      <c r="I6" s="8">
         <v>4.9400000000000004</v>
       </c>
-      <c r="I6" s="8">
+      <c r="J6" s="8">
         <v>2.06</v>
       </c>
-      <c r="J6" s="8">
+      <c r="K6" s="8">
         <v>0</v>
       </c>
-      <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>18</v>
       </c>
@@ -978,32 +1028,36 @@
         <f>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</f>
         <v>1.0630145812734651E-8</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="14">
+        <f>Table1[[#This Row],[Int ratio]]</f>
+        <v>1.0630145812734651E-8</v>
+      </c>
+      <c r="F7" s="9">
         <v>3.39E-4</v>
       </c>
-      <c r="F7" s="9">
+      <c r="G7" s="9">
         <v>7.4599999999999996E-3</v>
       </c>
-      <c r="G7" s="9">
+      <c r="H7" s="9">
         <v>-7.45E-3</v>
       </c>
-      <c r="H7" s="8">
+      <c r="I7" s="8">
         <v>4.84</v>
       </c>
-      <c r="I7" s="8">
+      <c r="J7" s="8">
         <v>2.0099999999999998</v>
       </c>
-      <c r="J7" s="8">
+      <c r="K7" s="8">
         <v>0</v>
       </c>
-      <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>19</v>
       </c>
@@ -1017,32 +1071,36 @@
         <f>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</f>
         <v>1.053565375285274E-8</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="14">
+        <f>Table1[[#This Row],[Int ratio]]</f>
+        <v>1.053565375285274E-8</v>
+      </c>
+      <c r="F8" s="9">
         <v>-3.9199999999999999E-4</v>
       </c>
-      <c r="F8" s="9">
+      <c r="G8" s="9">
         <v>6.8500000000000002E-3</v>
       </c>
-      <c r="G8" s="9">
+      <c r="H8" s="9">
         <v>-6.8399999999999997E-3</v>
       </c>
-      <c r="H8" s="8">
+      <c r="I8" s="8">
         <v>4.7699999999999996</v>
       </c>
-      <c r="I8" s="8">
+      <c r="J8" s="8">
         <v>1.98</v>
       </c>
-      <c r="J8" s="8">
+      <c r="K8" s="8">
         <v>0</v>
       </c>
-      <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>19.100000000000001</v>
       </c>
@@ -1056,32 +1114,36 @@
         <f>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</f>
         <v>1.0488088481701517E-8</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="14">
+        <f>Table1[[#This Row],[Int ratio]]</f>
+        <v>1.0488088481701517E-8</v>
+      </c>
+      <c r="F9" s="9">
         <v>-6.0099999999999997E-4</v>
       </c>
-      <c r="F9" s="9">
+      <c r="G9" s="9">
         <v>6.7600000000000004E-3</v>
       </c>
-      <c r="G9" s="9">
+      <c r="H9" s="9">
         <v>-6.7299999999999999E-3</v>
       </c>
-      <c r="H9" s="8">
+      <c r="I9" s="8">
         <v>4.76</v>
       </c>
-      <c r="I9" s="8">
+      <c r="J9" s="8">
         <v>1.98</v>
       </c>
-      <c r="J9" s="8">
+      <c r="K9" s="8">
         <v>0</v>
       </c>
-      <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-    </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q9" s="5"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="11">
         <v>19.5</v>
       </c>
@@ -1095,32 +1157,36 @@
         <f>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</f>
         <v>1.067707825203131E-8</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="13">
+        <f>Table1[[#This Row],[Int ratio]]</f>
+        <v>1.067707825203131E-8</v>
+      </c>
+      <c r="F10" s="8">
         <v>-1.0200000000000001E-3</v>
       </c>
-      <c r="F10" s="8">
+      <c r="G10" s="8">
         <v>6.6899999999999998E-3</v>
       </c>
-      <c r="G10" s="8">
+      <c r="H10" s="8">
         <v>-6.6100000000000004E-3</v>
       </c>
-      <c r="H10" s="8">
+      <c r="I10" s="8">
         <v>4.7300000000000004</v>
       </c>
-      <c r="I10" s="8">
+      <c r="J10" s="8">
         <v>1.97</v>
       </c>
-      <c r="J10" s="8">
+      <c r="K10" s="8">
         <v>0</v>
       </c>
-      <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-    </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q10" s="5"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="11">
         <v>20.100000000000001</v>
       </c>
@@ -1134,84 +1200,88 @@
         <f>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</f>
         <v>1.1704699910719625E-8</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="13">
+        <f>Table1[[#This Row],[Int ratio]]</f>
+        <v>1.1704699910719625E-8</v>
+      </c>
+      <c r="F11" s="8">
         <v>-2.1099999999999999E-3</v>
       </c>
-      <c r="F11" s="8">
+      <c r="G11" s="8">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G11" s="8">
+      <c r="H11" s="8">
         <v>-6.6800000000000002E-3</v>
       </c>
-      <c r="H11" s="8">
+      <c r="I11" s="8">
         <v>4.6900000000000004</v>
       </c>
-      <c r="I11" s="8">
+      <c r="J11" s="8">
         <v>1.95</v>
       </c>
-      <c r="J11" s="8">
+      <c r="K11" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K13" s="1"/>
-      <c r="L13" s="2"/>
+    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L13" s="1"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
-      <c r="Q13" s="5"/>
+      <c r="Q13" s="2"/>
       <c r="R13" s="5"/>
-    </row>
-    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K14" s="1"/>
-      <c r="L14" s="2"/>
+      <c r="S13" s="5"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L14" s="1"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
-      <c r="Q14" s="5"/>
+      <c r="Q14" s="2"/>
       <c r="R14" s="5"/>
-    </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K15" s="1"/>
-      <c r="L15" s="2"/>
+      <c r="S14" s="5"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L15" s="1"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
-      <c r="Q15" s="5"/>
+      <c r="Q15" s="2"/>
       <c r="R15" s="5"/>
-    </row>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K16" s="1"/>
-      <c r="L16" s="2"/>
+      <c r="S15" s="5"/>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L16" s="1"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
-      <c r="Q16" s="5"/>
+      <c r="Q16" s="2"/>
       <c r="R16" s="5"/>
-    </row>
-    <row r="17" spans="11:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K17" s="1"/>
-      <c r="L17" s="2"/>
+      <c r="S16" s="5"/>
+    </row>
+    <row r="17" spans="12:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L17" s="1"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
-      <c r="Q17" s="5"/>
+      <c r="Q17" s="2"/>
       <c r="R17" s="5"/>
-    </row>
-    <row r="18" spans="11:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K18" s="1"/>
-      <c r="L18" s="2"/>
+      <c r="S17" s="5"/>
+    </row>
+    <row r="18" spans="12:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L18" s="1"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
-      <c r="Q18" s="5"/>
+      <c r="Q18" s="2"/>
       <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>